<commit_message>
whatever a pk1 is
</commit_message>
<xml_diff>
--- a/3_Data_Analysis/performance_analysis_results/error_details.xlsx
+++ b/3_Data_Analysis/performance_analysis_results/error_details.xlsx
@@ -11,9 +11,9 @@
     <sheet name="Left_Lower_Face_Paralysis" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Right_Upper_Face_Paralysis" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Right_Mid_Face_Paralysis" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="OralOcular_Right" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="OcularOral_Left" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="OcularOral_Right" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="OralOcular_Left" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="OralOcular_Right" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="OcularOral_Left" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="SnarlSmile_Left" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="SnarlSmile_Right" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Mentalis_Left" sheetId="10" state="visible" r:id="rId10"/>
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_2259</t>
+          <t>IMG_0490</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,7 +605,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IMG_2737</t>
+          <t>IMG_2814</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -622,100 +622,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IMG_3102</t>
+          <t>IMG_3324</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IMG_3324</t>
+          <t>IMG_8537</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>IMG_3812</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>IMG_4923</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>IMG_5694</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>IMG_7365</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -732,7 +664,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -760,7 +692,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_3170</t>
+          <t>IMG_2737</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -788,6 +720,23 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>IMG_9640</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -830,7 +779,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_3847</t>
+          <t>IMG_1339</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -847,7 +796,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IMG_8537</t>
+          <t>IMG_3847</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1031,7 +980,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1059,7 +1008,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_0490</t>
+          <t>IMG_9330</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1068,23 +1017,6 @@
         </is>
       </c>
       <c r="C2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>IMG_5694</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1129,7 +1061,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_3812</t>
+          <t>IMG_4923</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1146,17 +1078,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IMG_4210</t>
+          <t>IMG_5694</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1131,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_7365</t>
+          <t>IMG_2068</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1224,7 +1156,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1252,24 +1184,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_0495</t>
+          <t>IMG_0504</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IMG_2814</t>
+          <t>IMG_7365</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1286,17 +1218,34 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IMG_5694</t>
+          <t>IMG_8514</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>IMG_9374</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1260,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1339,7 +1288,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_0495</t>
+          <t>IMG_4157</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1350,74 +1299,6 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>IMG_2122</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>IMG_2501</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>IMG_4210</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>IMG_7365</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>